<commit_message>
tested sim with different input voltages
</commit_message>
<xml_diff>
--- a/DC_Converter_Calc.xlsx
+++ b/DC_Converter_Calc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BR\GIT\HV_DCDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B693AE64-768A-4D68-A7DA-25EC8594D99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946273A1-4D61-499D-9898-6605F9612C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2490" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -182,7 +182,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -229,7 +229,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -655,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="Y38" sqref="Y38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,8 +799,8 @@
         <v>17</v>
       </c>
       <c r="B15" s="3">
-        <f>1/0.182</f>
-        <v>5.4945054945054945</v>
+        <f>F17</f>
+        <v>12.048192771084336</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -813,7 +813,8 @@
         <v>13</v>
       </c>
       <c r="B17">
-        <v>2600</v>
+        <f>F18</f>
+        <v>3100</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
@@ -840,7 +841,7 @@
       </c>
       <c r="B18" s="3">
         <f>B17/(B15^2)</f>
-        <v>86.122399999999999</v>
+        <v>21.355900000000005</v>
       </c>
       <c r="C18" t="s">
         <v>15</v>
@@ -888,14 +889,14 @@
       </c>
       <c r="B22" s="2">
         <f>(1-((1/B5)*B15*B3))*1/B21*B3*1/B9</f>
-        <v>3.3741539359516896E-5</v>
+        <v>-6.4240619269724338E-6</v>
       </c>
       <c r="C22" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="3">
         <f>B22*10^6</f>
-        <v>33.741539359516892</v>
+        <v>-6.4240619269724339</v>
       </c>
       <c r="E22" t="s">
         <v>15</v>
@@ -907,14 +908,14 @@
       </c>
       <c r="B23" s="2">
         <f>(1-((1/B6)*B15*B3))*1/B21*B3*1/B9</f>
-        <v>5.1569052229990773E-5</v>
+        <v>3.2667592801054613E-5</v>
       </c>
       <c r="C23" t="s">
         <v>27</v>
       </c>
       <c r="D23" s="3">
         <f>B23*10^6</f>
-        <v>51.569052229990774</v>
+        <v>32.66759280105461</v>
       </c>
       <c r="E23" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Added IC's and Mosfets on the Schematic with complementary circuit
</commit_message>
<xml_diff>
--- a/DC_Converter_Calc.xlsx
+++ b/DC_Converter_Calc.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Technik\Technik 2022\05 - Electronics\02 - HV\01 - HV Accumulator\02 - ECAD\02 - PCB Files\03 - HV_DCDC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BR\GIT\HV_DCDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC7B285-3175-4BB5-9AF1-325C01EA9841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35094DE7-FDC1-452C-B9B4-5B58EE2715B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="26760" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="154">
   <si>
     <t>Eingangsparameter</t>
   </si>
@@ -464,6 +466,36 @@
   </si>
   <si>
     <t xml:space="preserve">IXFK240N25X3 </t>
+  </si>
+  <si>
+    <t>Housekeeping Mosfet</t>
+  </si>
+  <si>
+    <t>Based on refernece design BSP300</t>
+  </si>
+  <si>
+    <t>190mA</t>
+  </si>
+  <si>
+    <t>R_ds_on</t>
+  </si>
+  <si>
+    <t>N_channel</t>
+  </si>
+  <si>
+    <t>V_DS</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>I_cont</t>
+  </si>
+  <si>
+    <t>1,85A</t>
+  </si>
+  <si>
+    <t>N_Channel</t>
   </si>
 </sst>
 </file>
@@ -570,14 +602,14 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -744,9 +776,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>512444</xdr:colOff>
+      <xdr:colOff>516254</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>91749</xdr:rowOff>
+      <xdr:rowOff>95559</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -790,7 +822,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>190499</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>170421</xdr:rowOff>
+      <xdr:rowOff>174231</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -832,9 +864,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>554903</xdr:colOff>
+      <xdr:colOff>551093</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -876,9 +908,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>14911</xdr:colOff>
+      <xdr:colOff>18721</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>160864</xdr:rowOff>
+      <xdr:rowOff>168484</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -922,7 +954,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>610916</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>178426</xdr:rowOff>
+      <xdr:rowOff>174616</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -964,9 +996,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>139328</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>186384</xdr:rowOff>
+      <xdr:colOff>135518</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>548</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1008,9 +1040,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>242126</xdr:colOff>
+      <xdr:colOff>245936</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>144517</xdr:rowOff>
+      <xdr:rowOff>136897</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1052,9 +1084,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>772707</xdr:colOff>
+      <xdr:colOff>782232</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>169839</xdr:rowOff>
+      <xdr:rowOff>173649</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1096,9 +1128,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>18197</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>186300</xdr:rowOff>
+      <xdr:colOff>22007</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>464</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1140,9 +1172,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>95248</xdr:colOff>
+      <xdr:colOff>99058</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>167720</xdr:rowOff>
+      <xdr:rowOff>171530</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1549,37 +1581,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X98"/>
+  <dimension ref="A1:X105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61:I64"/>
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
       <c r="J1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1590,7 +1622,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1607,7 +1639,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1621,7 +1653,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1638,7 +1670,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1652,7 +1684,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1664,7 +1696,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1679,7 +1711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -1690,7 +1722,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -1701,23 +1733,23 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="20"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1734,7 +1766,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1745,7 +1777,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1761,7 +1793,7 @@
         <v>6.708333333333333</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1770,7 +1802,7 @@
         <v>10.989010989010989</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1789,7 +1821,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E20" t="s">
         <v>18</v>
       </c>
@@ -1800,7 +1832,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1831,7 +1863,7 @@
         <v>10.989010989010989</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -1858,7 +1890,7 @@
         <v>3900</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
         <v>35</v>
       </c>
@@ -1875,7 +1907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -1886,7 +1918,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1895,20 +1927,20 @@
         <v>0.99923076923076926</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1920,7 +1952,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -1932,7 +1964,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1951,7 +1983,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1970,7 +2002,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>25</v>
       </c>
@@ -1990,10 +2022,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:24" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -2011,7 +2043,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:24" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -2020,7 +2052,7 @@
       </c>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:24" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -2042,7 +2074,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -2061,7 +2093,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -2079,7 +2111,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -2091,7 +2123,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -2103,7 +2135,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -2143,7 +2175,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -2181,18 +2213,18 @@
         <v>101</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A45" s="29" t="s">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A45" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="29"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="31"/>
+      <c r="H45" s="31"/>
+      <c r="I45" s="31"/>
       <c r="R45" t="s">
         <v>95</v>
       </c>
@@ -2206,7 +2238,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -2226,7 +2258,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -2257,7 +2289,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -2285,7 +2317,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -2294,7 +2326,7 @@
         <v>0.5733397037744864</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -2306,7 +2338,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>71</v>
       </c>
@@ -2318,20 +2350,20 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A54" s="29" t="s">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A54" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="B54" s="29"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="29"/>
-      <c r="H54" s="29"/>
-      <c r="I54" s="29"/>
-    </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B54" s="31"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="31"/>
+      <c r="H54" s="31"/>
+      <c r="I54" s="31"/>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>81</v>
       </c>
@@ -2346,7 +2378,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>73</v>
       </c>
@@ -2360,7 +2392,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>74</v>
       </c>
@@ -2378,7 +2410,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>72</v>
       </c>
@@ -2403,7 +2435,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>87</v>
       </c>
@@ -2415,14 +2447,14 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="G61" s="30" t="s">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="G61" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="H61" s="31"/>
-      <c r="I61" s="31"/>
-    </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="H61" s="30"/>
+      <c r="I61" s="30"/>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>77</v>
       </c>
@@ -2432,11 +2464,11 @@
       <c r="C62" t="s">
         <v>79</v>
       </c>
-      <c r="G62" s="31"/>
-      <c r="H62" s="31"/>
-      <c r="I62" s="31"/>
-    </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G62" s="30"/>
+      <c r="H62" s="30"/>
+      <c r="I62" s="30"/>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>78</v>
       </c>
@@ -2446,9 +2478,9 @@
       <c r="C63" t="s">
         <v>10</v>
       </c>
-      <c r="G63" s="31"/>
-      <c r="H63" s="31"/>
-      <c r="I63" s="31"/>
+      <c r="G63" s="30"/>
+      <c r="H63" s="30"/>
+      <c r="I63" s="30"/>
       <c r="R63" t="s">
         <v>93</v>
       </c>
@@ -2468,7 +2500,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>76</v>
       </c>
@@ -2486,9 +2518,9 @@
       <c r="E64" t="s">
         <v>75</v>
       </c>
-      <c r="G64" s="31"/>
-      <c r="H64" s="31"/>
-      <c r="I64" s="31"/>
+      <c r="G64" s="30"/>
+      <c r="H64" s="30"/>
+      <c r="I64" s="30"/>
       <c r="R64" t="s">
         <v>94</v>
       </c>
@@ -2508,7 +2540,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>89</v>
       </c>
@@ -2541,7 +2573,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
       <c r="R66" t="s">
         <v>96</v>
       </c>
@@ -2552,7 +2584,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>80</v>
       </c>
@@ -2576,7 +2608,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>84</v>
       </c>
@@ -2613,12 +2645,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D69" s="27"/>
       <c r="E69" s="20"/>
       <c r="F69" s="20"/>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>138</v>
       </c>
@@ -2633,7 +2665,7 @@
       <c r="E70" s="20"/>
       <c r="F70" s="20"/>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>122</v>
       </c>
@@ -2652,7 +2684,7 @@
       </c>
       <c r="F71" s="20"/>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>140</v>
       </c>
@@ -2667,20 +2699,20 @@
       <c r="E72" s="20"/>
       <c r="F72" s="20"/>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A74" s="29" t="s">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A74" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="B74" s="29"/>
-      <c r="C74" s="29"/>
-      <c r="D74" s="29"/>
-      <c r="E74" s="29"/>
-      <c r="F74" s="29"/>
-      <c r="G74" s="29"/>
-      <c r="H74" s="29"/>
-      <c r="I74" s="29"/>
-    </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B74" s="31"/>
+      <c r="C74" s="31"/>
+      <c r="D74" s="31"/>
+      <c r="E74" s="31"/>
+      <c r="F74" s="31"/>
+      <c r="G74" s="31"/>
+      <c r="H74" s="31"/>
+      <c r="I74" s="31"/>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>114</v>
       </c>
@@ -2691,12 +2723,12 @@
       <c r="C75" t="s">
         <v>23</v>
       </c>
-      <c r="F75" s="31" t="s">
+      <c r="F75" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="G75" s="31"/>
-    </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="G75" s="30"/>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>116</v>
       </c>
@@ -2707,10 +2739,10 @@
       <c r="D76" t="s">
         <v>117</v>
       </c>
-      <c r="F76" s="31"/>
-      <c r="G76" s="31"/>
-    </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F76" s="30"/>
+      <c r="G76" s="30"/>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>115</v>
       </c>
@@ -2721,23 +2753,23 @@
       <c r="C77" t="s">
         <v>23</v>
       </c>
-      <c r="F77" s="31"/>
-      <c r="G77" s="31"/>
-    </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A78" s="29" t="s">
+      <c r="F77" s="30"/>
+      <c r="G77" s="30"/>
+    </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A78" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="B78" s="29"/>
-      <c r="C78" s="29"/>
-      <c r="D78" s="29"/>
-      <c r="E78" s="29"/>
-      <c r="F78" s="29"/>
-      <c r="G78" s="29"/>
-      <c r="H78" s="29"/>
-      <c r="I78" s="29"/>
-    </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B78" s="31"/>
+      <c r="C78" s="31"/>
+      <c r="D78" s="31"/>
+      <c r="E78" s="31"/>
+      <c r="F78" s="31"/>
+      <c r="G78" s="31"/>
+      <c r="H78" s="31"/>
+      <c r="I78" s="31"/>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>118</v>
       </c>
@@ -2749,7 +2781,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>119</v>
       </c>
@@ -2761,7 +2793,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>74</v>
       </c>
@@ -2771,12 +2803,12 @@
       <c r="C81" t="s">
         <v>42</v>
       </c>
-      <c r="F81" s="31" t="s">
+      <c r="F81" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="G81" s="31"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G81" s="30"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>122</v>
       </c>
@@ -2793,10 +2825,10 @@
       <c r="E82" t="s">
         <v>124</v>
       </c>
-      <c r="F82" s="31"/>
-      <c r="G82" s="31"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F82" s="30"/>
+      <c r="G82" s="30"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>128</v>
       </c>
@@ -2813,10 +2845,10 @@
       <c r="E83" t="s">
         <v>124</v>
       </c>
-      <c r="F83" s="31"/>
-      <c r="G83" s="31"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F83" s="30"/>
+      <c r="G83" s="30"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>120</v>
       </c>
@@ -2828,7 +2860,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>121</v>
       </c>
@@ -2840,7 +2872,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>126</v>
       </c>
@@ -2852,7 +2884,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>127</v>
       </c>
@@ -2864,7 +2896,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>129</v>
       </c>
@@ -2876,20 +2908,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="29" t="s">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A90" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="B90" s="29"/>
-      <c r="C90" s="29"/>
-      <c r="D90" s="29"/>
-      <c r="E90" s="29"/>
-      <c r="F90" s="29"/>
-      <c r="G90" s="29"/>
-      <c r="H90" s="29"/>
-      <c r="I90" s="29"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B90" s="31"/>
+      <c r="C90" s="31"/>
+      <c r="D90" s="31"/>
+      <c r="E90" s="31"/>
+      <c r="F90" s="31"/>
+      <c r="G90" s="31"/>
+      <c r="H90" s="31"/>
+      <c r="I90" s="31"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>135</v>
       </c>
@@ -2904,7 +2936,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>135</v>
       </c>
@@ -2919,7 +2951,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>138</v>
       </c>
@@ -2931,13 +2963,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F94" s="31" t="s">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F94" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="G94" s="31"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G94" s="30"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>74</v>
       </c>
@@ -2954,10 +2986,10 @@
       <c r="E95" t="s">
         <v>43</v>
       </c>
-      <c r="F95" s="31"/>
-      <c r="G95" s="31"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F95" s="30"/>
+      <c r="G95" s="30"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>122</v>
       </c>
@@ -2974,10 +3006,10 @@
       <c r="E96" t="s">
         <v>124</v>
       </c>
-      <c r="F96" s="31"/>
-      <c r="G96" s="31"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F96" s="30"/>
+      <c r="G96" s="30"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>139</v>
       </c>
@@ -2989,8 +3021,76 @@
         <v>20</v>
       </c>
     </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A100" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B100" s="31"/>
+      <c r="C100" s="31"/>
+      <c r="D100" s="31"/>
+      <c r="E100" s="31"/>
+      <c r="F100" s="31"/>
+      <c r="G100" s="31"/>
+      <c r="H100" s="31"/>
+      <c r="I100" s="31"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>151</v>
+      </c>
+      <c r="B102" t="s">
+        <v>146</v>
+      </c>
+      <c r="C102" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>147</v>
+      </c>
+      <c r="B103">
+        <v>15</v>
+      </c>
+      <c r="C103">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>150</v>
+      </c>
+      <c r="B104" t="s">
+        <v>148</v>
+      </c>
+      <c r="C104" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>149</v>
+      </c>
+      <c r="B105">
+        <v>800</v>
+      </c>
+      <c r="C105">
+        <v>1000</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="A100:I100"/>
+    <mergeCell ref="A45:I45"/>
+    <mergeCell ref="A13:I13"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A54:I54"/>
+    <mergeCell ref="A1:I1"/>
     <mergeCell ref="G61:I64"/>
     <mergeCell ref="A90:I90"/>
     <mergeCell ref="F94:G96"/>
@@ -2998,11 +3098,6 @@
     <mergeCell ref="A78:I78"/>
     <mergeCell ref="F81:G83"/>
     <mergeCell ref="F75:G77"/>
-    <mergeCell ref="A45:I45"/>
-    <mergeCell ref="A13:I13"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A54:I54"/>
-    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Put most parts on schematic and wired the up
Still most need values
and a few complementary circuits
</commit_message>
<xml_diff>
--- a/DC_Converter_Calc.xlsx
+++ b/DC_Converter_Calc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BR\GIT\HV_DCDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35094DE7-FDC1-452C-B9B4-5B58EE2715B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C4E90E-DF52-4E4A-8FE7-9B1E811BEC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="26760" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -602,14 +602,14 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1583,8 +1583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D106" sqref="D106"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1596,17 +1596,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
       <c r="J1" t="s">
         <v>58</v>
       </c>
@@ -1737,17 +1737,17 @@
       <c r="B12" s="20"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1928,17 +1928,17 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -2214,17 +2214,17 @@
       </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A45" s="31" t="s">
+      <c r="A45" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="B45" s="31"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="31"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
       <c r="R45" t="s">
         <v>95</v>
       </c>
@@ -2351,17 +2351,17 @@
       </c>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A54" s="31" t="s">
+      <c r="A54" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="B54" s="31"/>
-      <c r="C54" s="31"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="31"/>
-      <c r="H54" s="31"/>
-      <c r="I54" s="31"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="29"/>
+      <c r="H54" s="29"/>
+      <c r="I54" s="29"/>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
@@ -2448,11 +2448,11 @@
       </c>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="G61" s="29" t="s">
+      <c r="G61" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="H61" s="30"/>
-      <c r="I61" s="30"/>
+      <c r="H61" s="31"/>
+      <c r="I61" s="31"/>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
@@ -2464,9 +2464,9 @@
       <c r="C62" t="s">
         <v>79</v>
       </c>
-      <c r="G62" s="30"/>
-      <c r="H62" s="30"/>
-      <c r="I62" s="30"/>
+      <c r="G62" s="31"/>
+      <c r="H62" s="31"/>
+      <c r="I62" s="31"/>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
@@ -2478,9 +2478,9 @@
       <c r="C63" t="s">
         <v>10</v>
       </c>
-      <c r="G63" s="30"/>
-      <c r="H63" s="30"/>
-      <c r="I63" s="30"/>
+      <c r="G63" s="31"/>
+      <c r="H63" s="31"/>
+      <c r="I63" s="31"/>
       <c r="R63" t="s">
         <v>93</v>
       </c>
@@ -2518,9 +2518,9 @@
       <c r="E64" t="s">
         <v>75</v>
       </c>
-      <c r="G64" s="30"/>
-      <c r="H64" s="30"/>
-      <c r="I64" s="30"/>
+      <c r="G64" s="31"/>
+      <c r="H64" s="31"/>
+      <c r="I64" s="31"/>
       <c r="R64" t="s">
         <v>94</v>
       </c>
@@ -2700,17 +2700,17 @@
       <c r="F72" s="20"/>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A74" s="31" t="s">
+      <c r="A74" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="B74" s="31"/>
-      <c r="C74" s="31"/>
-      <c r="D74" s="31"/>
-      <c r="E74" s="31"/>
-      <c r="F74" s="31"/>
-      <c r="G74" s="31"/>
-      <c r="H74" s="31"/>
-      <c r="I74" s="31"/>
+      <c r="B74" s="29"/>
+      <c r="C74" s="29"/>
+      <c r="D74" s="29"/>
+      <c r="E74" s="29"/>
+      <c r="F74" s="29"/>
+      <c r="G74" s="29"/>
+      <c r="H74" s="29"/>
+      <c r="I74" s="29"/>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
@@ -2723,10 +2723,10 @@
       <c r="C75" t="s">
         <v>23</v>
       </c>
-      <c r="F75" s="30" t="s">
+      <c r="F75" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G75" s="30"/>
+      <c r="G75" s="31"/>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
@@ -2739,8 +2739,8 @@
       <c r="D76" t="s">
         <v>117</v>
       </c>
-      <c r="F76" s="30"/>
-      <c r="G76" s="30"/>
+      <c r="F76" s="31"/>
+      <c r="G76" s="31"/>
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
@@ -2753,21 +2753,21 @@
       <c r="C77" t="s">
         <v>23</v>
       </c>
-      <c r="F77" s="30"/>
-      <c r="G77" s="30"/>
+      <c r="F77" s="31"/>
+      <c r="G77" s="31"/>
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A78" s="31" t="s">
+      <c r="A78" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="B78" s="31"/>
-      <c r="C78" s="31"/>
-      <c r="D78" s="31"/>
-      <c r="E78" s="31"/>
-      <c r="F78" s="31"/>
-      <c r="G78" s="31"/>
-      <c r="H78" s="31"/>
-      <c r="I78" s="31"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="29"/>
+      <c r="D78" s="29"/>
+      <c r="E78" s="29"/>
+      <c r="F78" s="29"/>
+      <c r="G78" s="29"/>
+      <c r="H78" s="29"/>
+      <c r="I78" s="29"/>
     </row>
     <row r="79" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
@@ -2803,10 +2803,10 @@
       <c r="C81" t="s">
         <v>42</v>
       </c>
-      <c r="F81" s="30" t="s">
+      <c r="F81" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="G81" s="30"/>
+      <c r="G81" s="31"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
@@ -2825,8 +2825,8 @@
       <c r="E82" t="s">
         <v>124</v>
       </c>
-      <c r="F82" s="30"/>
-      <c r="G82" s="30"/>
+      <c r="F82" s="31"/>
+      <c r="G82" s="31"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
@@ -2845,8 +2845,8 @@
       <c r="E83" t="s">
         <v>124</v>
       </c>
-      <c r="F83" s="30"/>
-      <c r="G83" s="30"/>
+      <c r="F83" s="31"/>
+      <c r="G83" s="31"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
@@ -2909,17 +2909,17 @@
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90" s="31" t="s">
+      <c r="A90" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="B90" s="31"/>
-      <c r="C90" s="31"/>
-      <c r="D90" s="31"/>
-      <c r="E90" s="31"/>
-      <c r="F90" s="31"/>
-      <c r="G90" s="31"/>
-      <c r="H90" s="31"/>
-      <c r="I90" s="31"/>
+      <c r="B90" s="29"/>
+      <c r="C90" s="29"/>
+      <c r="D90" s="29"/>
+      <c r="E90" s="29"/>
+      <c r="F90" s="29"/>
+      <c r="G90" s="29"/>
+      <c r="H90" s="29"/>
+      <c r="I90" s="29"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
@@ -2964,10 +2964,10 @@
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F94" s="30" t="s">
+      <c r="F94" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="G94" s="30"/>
+      <c r="G94" s="31"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
@@ -2986,8 +2986,8 @@
       <c r="E95" t="s">
         <v>43</v>
       </c>
-      <c r="F95" s="30"/>
-      <c r="G95" s="30"/>
+      <c r="F95" s="31"/>
+      <c r="G95" s="31"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
@@ -3006,8 +3006,8 @@
       <c r="E96" t="s">
         <v>124</v>
       </c>
-      <c r="F96" s="30"/>
-      <c r="G96" s="30"/>
+      <c r="F96" s="31"/>
+      <c r="G96" s="31"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
@@ -3022,17 +3022,17 @@
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" s="31" t="s">
+      <c r="A100" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="B100" s="31"/>
-      <c r="C100" s="31"/>
-      <c r="D100" s="31"/>
-      <c r="E100" s="31"/>
-      <c r="F100" s="31"/>
-      <c r="G100" s="31"/>
-      <c r="H100" s="31"/>
-      <c r="I100" s="31"/>
+      <c r="B100" s="29"/>
+      <c r="C100" s="29"/>
+      <c r="D100" s="29"/>
+      <c r="E100" s="29"/>
+      <c r="F100" s="29"/>
+      <c r="G100" s="29"/>
+      <c r="H100" s="29"/>
+      <c r="I100" s="29"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
@@ -3085,11 +3085,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A100:I100"/>
-    <mergeCell ref="A45:I45"/>
-    <mergeCell ref="A13:I13"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A54:I54"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="G61:I64"/>
     <mergeCell ref="A90:I90"/>
@@ -3098,6 +3093,11 @@
     <mergeCell ref="A78:I78"/>
     <mergeCell ref="F81:G83"/>
     <mergeCell ref="F75:G77"/>
+    <mergeCell ref="A100:I100"/>
+    <mergeCell ref="A45:I45"/>
+    <mergeCell ref="A13:I13"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A54:I54"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added and imprioved on cooler calcualtion for mosfets
</commit_message>
<xml_diff>
--- a/DC_Converter_Calc.xlsx
+++ b/DC_Converter_Calc.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BR\GIT\HV_DCDC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Technik\Technik 2022\05 - Electronics\02 - HV\01 - HV Accumulator\02 - ECAD\02 - PCB Files\03 - HV_DCDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C04A78E-BEF6-4E8A-B0AA-1C49B896F308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB66EDD-EFD3-4C51-BDBE-4BCD818C69D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="183">
   <si>
     <t>Eingangsparameter</t>
   </si>
@@ -550,9 +548,6 @@
     <t>W/K</t>
   </si>
   <si>
-    <t>WA-T264-101E</t>
-  </si>
-  <si>
     <t>geschätzt</t>
   </si>
   <si>
@@ -569,6 +564,24 @@
   </si>
   <si>
     <t>WA-T220-101E</t>
+  </si>
+  <si>
+    <t>I_D_Max_pulsed</t>
+  </si>
+  <si>
+    <t>P_ACM_Max</t>
+  </si>
+  <si>
+    <t>Safety Factor</t>
+  </si>
+  <si>
+    <t>T_th_gesamt</t>
+  </si>
+  <si>
+    <t>t_max</t>
+  </si>
+  <si>
+    <t>CR101-75</t>
   </si>
 </sst>
 </file>
@@ -666,7 +679,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -714,7 +727,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -722,9 +741,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1332,7 +1348,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="14695552"/>
@@ -1393,7 +1409,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="10189344"/>
@@ -1435,7 +1451,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2037159264"/>
@@ -1501,7 +1517,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2638,13 +2654,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>67235</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>179294</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>582706</xdr:colOff>
-      <xdr:row>102</xdr:row>
+      <xdr:row>108</xdr:row>
       <xdr:rowOff>78441</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2746,13 +2762,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>66261</xdr:colOff>
-      <xdr:row>98</xdr:row>
+      <xdr:row>104</xdr:row>
       <xdr:rowOff>162340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>371061</xdr:colOff>
-      <xdr:row>123</xdr:row>
+      <xdr:row>132</xdr:row>
       <xdr:rowOff>122583</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3137,37 +3153,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X145"/>
+  <dimension ref="A1:X157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H95" sqref="H95"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O80" sqref="O80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
       <c r="J1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3178,7 +3194,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3195,7 +3211,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -3209,7 +3225,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -3226,7 +3242,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -3240,7 +3256,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -3252,7 +3268,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -3267,7 +3283,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -3278,7 +3294,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -3289,10 +3305,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="20"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>157</v>
       </c>
@@ -3303,7 +3319,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>160</v>
       </c>
@@ -3314,20 +3330,20 @@
         <v>158</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="45" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="45"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="46"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -3344,7 +3360,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -3355,7 +3371,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -3371,7 +3387,7 @@
         <v>6.708333333333333</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -3380,7 +3396,7 @@
         <v>10.989010989010989</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -3399,7 +3415,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
         <v>18</v>
       </c>
@@ -3410,7 +3426,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -3441,7 +3457,7 @@
         <v>10.989010989010989</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -3468,7 +3484,7 @@
         <v>3900</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
         <v>35</v>
       </c>
@@ -3485,7 +3501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -3496,7 +3512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -3505,20 +3521,20 @@
         <v>0.99923076923076926</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="45" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -3530,7 +3546,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -3542,7 +3558,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -3561,7 +3577,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -3580,7 +3596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>25</v>
       </c>
@@ -3603,10 +3619,10 @@
         <v>156</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" ht="15.75" x14ac:dyDescent="0.3">
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>61</v>
       </c>
@@ -3624,7 +3640,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>64</v>
       </c>
@@ -3633,7 +3649,7 @@
       </c>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -3655,7 +3671,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -3674,7 +3690,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -3692,7 +3708,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -3704,7 +3720,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -3716,7 +3732,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -3756,7 +3772,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -3794,18 +3810,18 @@
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A47" s="45" t="s">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A47" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="45"/>
+      <c r="B47" s="46"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="46"/>
+      <c r="I47" s="46"/>
       <c r="R47" t="s">
         <v>95</v>
       </c>
@@ -3819,7 +3835,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -3839,7 +3855,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -3870,7 +3886,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -3898,7 +3914,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -3907,7 +3923,7 @@
         <v>0.5733397037744864</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -3919,7 +3935,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>71</v>
       </c>
@@ -3931,20 +3947,20 @@
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A56" s="45" t="s">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A56" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="B56" s="45"/>
-      <c r="C56" s="45"/>
-      <c r="D56" s="45"/>
-      <c r="E56" s="45"/>
-      <c r="F56" s="45"/>
-      <c r="G56" s="45"/>
-      <c r="H56" s="45"/>
-      <c r="I56" s="45"/>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B56" s="46"/>
+      <c r="C56" s="46"/>
+      <c r="D56" s="46"/>
+      <c r="E56" s="46"/>
+      <c r="F56" s="46"/>
+      <c r="G56" s="46"/>
+      <c r="H56" s="46"/>
+      <c r="I56" s="46"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>81</v>
       </c>
@@ -3959,7 +3975,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>73</v>
       </c>
@@ -3973,38 +3989,39 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>74</v>
       </c>
       <c r="B60" s="25">
         <f>D60*10^-3</f>
-        <v>4.0999999999999995E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="C60" t="s">
         <v>42</v>
       </c>
       <c r="D60" s="14">
-        <v>4.0999999999999996</v>
+        <f>5*1.6</f>
+        <v>8</v>
       </c>
       <c r="E60" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>72</v>
       </c>
       <c r="B61" s="7">
         <f>B58*B60</f>
-        <v>1.8449999999999998E-2</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="C61" t="s">
         <v>10</v>
       </c>
       <c r="D61" s="6">
         <f>B61*10^3</f>
-        <v>18.45</v>
+        <v>36.000000000000007</v>
       </c>
       <c r="E61" t="s">
         <v>75</v>
@@ -4016,26 +4033,26 @@
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>87</v>
       </c>
       <c r="B62" s="6">
         <f>D61*1.2</f>
-        <v>22.139999999999997</v>
+        <v>43.20000000000001</v>
       </c>
       <c r="C62" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="G63" s="46" t="s">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G63" s="48" t="s">
         <v>143</v>
       </c>
-      <c r="H63" s="47"/>
-      <c r="I63" s="47"/>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="H63" s="49"/>
+      <c r="I63" s="49"/>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>77</v>
       </c>
@@ -4045,11 +4062,11 @@
       <c r="C64" t="s">
         <v>79</v>
       </c>
-      <c r="G64" s="47"/>
-      <c r="H64" s="47"/>
-      <c r="I64" s="47"/>
-    </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="G64" s="49"/>
+      <c r="H64" s="49"/>
+      <c r="I64" s="49"/>
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>78</v>
       </c>
@@ -4059,11 +4076,11 @@
       <c r="C65" t="s">
         <v>10</v>
       </c>
-      <c r="G65" s="47"/>
-      <c r="H65" s="47"/>
-      <c r="I65" s="47"/>
+      <c r="G65" s="49"/>
+      <c r="H65" s="49"/>
+      <c r="I65" s="49"/>
       <c r="J65" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="R65" t="s">
         <v>93</v>
@@ -4084,27 +4101,27 @@
         <v>99</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>76</v>
       </c>
       <c r="B66" s="11">
         <f>B60*SQRT(2*B64*10^-3*((1.3*B65-B3)/(1.3*B65*B34*10^-6)))</f>
-        <v>1.0255255063149642</v>
+        <v>2.0010253781755405</v>
       </c>
       <c r="C66" t="s">
         <v>10</v>
       </c>
       <c r="D66">
         <f t="shared" ref="D66" si="0">B66*10^3</f>
-        <v>1025.5255063149641</v>
+        <v>2001.0253781755405</v>
       </c>
       <c r="E66" t="s">
         <v>75</v>
       </c>
-      <c r="G66" s="47"/>
-      <c r="H66" s="47"/>
-      <c r="I66" s="47"/>
+      <c r="G66" s="49"/>
+      <c r="H66" s="49"/>
+      <c r="I66" s="49"/>
       <c r="R66" t="s">
         <v>94</v>
       </c>
@@ -4124,13 +4141,13 @@
         <v>101</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>89</v>
       </c>
       <c r="B67" s="11">
         <f>B66/B60</f>
-        <v>250.12817227194253</v>
+        <v>250.12817227194256</v>
       </c>
       <c r="C67" t="s">
         <v>23</v>
@@ -4157,7 +4174,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="R68" t="s">
         <v>96</v>
       </c>
@@ -4168,7 +4185,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>80</v>
       </c>
@@ -4192,7 +4209,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>84</v>
       </c>
@@ -4229,12 +4246,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D71" s="27"/>
       <c r="E71" s="20"/>
       <c r="F71" s="20"/>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>138</v>
       </c>
@@ -4249,7 +4266,7 @@
       <c r="E72" s="20"/>
       <c r="F72" s="20"/>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>122</v>
       </c>
@@ -4268,13 +4285,13 @@
       </c>
       <c r="F73" s="20"/>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>140</v>
       </c>
       <c r="B74" s="22">
         <f>(B72^2*B60)+(B11*B9*B73)</f>
-        <v>5.5353206968149298</v>
+        <v>10.472455018175475</v>
       </c>
       <c r="C74" s="20" t="s">
         <v>20</v>
@@ -4283,22 +4300,22 @@
       <c r="E74" s="20"/>
       <c r="F74" s="20"/>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B75" s="22"/>
       <c r="C75" s="20"/>
       <c r="D75" s="27"/>
-      <c r="E75" s="48" t="s">
+      <c r="E75" s="47" t="s">
         <v>168</v>
       </c>
-      <c r="F75" s="48"/>
-    </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="F75" s="47"/>
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>159</v>
       </c>
       <c r="B76" s="22">
         <f>(B14-B13)/B74</f>
-        <v>13.549350454645859</v>
+        <v>7.1616445112281415</v>
       </c>
       <c r="C76" s="20" t="s">
         <v>161</v>
@@ -4311,7 +4328,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>162</v>
       </c>
@@ -4330,7 +4347,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>163</v>
       </c>
@@ -4349,7 +4366,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>164</v>
       </c>
@@ -4364,7 +4381,7 @@
       <c r="E79" s="20"/>
       <c r="F79" s="20"/>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>166</v>
       </c>
@@ -4379,13 +4396,13 @@
       <c r="E80" s="20"/>
       <c r="F80" s="20"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>167</v>
       </c>
       <c r="B81" s="22">
         <f>B76-B77-B78-B80</f>
-        <v>13.293707161558611</v>
+        <v>6.9060012181408936</v>
       </c>
       <c r="C81" s="20" t="s">
         <v>161</v>
@@ -4394,156 +4411,149 @@
       <c r="E81" s="20"/>
       <c r="F81" s="20"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B82" s="22"/>
       <c r="C82" s="20"/>
       <c r="D82" s="27"/>
       <c r="E82" s="20"/>
       <c r="F82" s="20"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="B83">
-        <v>11</v>
+        <v>4.2</v>
       </c>
       <c r="C83" s="20" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="45" t="s">
+      <c r="D83" s="27"/>
+      <c r="E83" s="20"/>
+      <c r="F83" s="20"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>180</v>
+      </c>
+      <c r="B84" s="21">
+        <f>B77+B78+B80+B83</f>
+        <v>4.455643293087248</v>
+      </c>
+      <c r="C84" s="20"/>
+      <c r="D84" s="27"/>
+      <c r="E84" s="20"/>
+      <c r="F84" s="20"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C85" s="20"/>
+      <c r="D85" s="27"/>
+      <c r="E85" s="20"/>
+      <c r="F85" s="20"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>181</v>
+      </c>
+      <c r="B86">
+        <f>B13+B74*B84</f>
+        <v>96.661523963891455</v>
+      </c>
+      <c r="C86" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="B84" s="45"/>
-      <c r="C84" s="45"/>
-      <c r="D84" s="45"/>
-      <c r="E84" s="45"/>
-      <c r="F84" s="45"/>
-      <c r="G84" s="45"/>
-      <c r="H84" s="45"/>
-      <c r="I84" s="45"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+      <c r="B87" s="46"/>
+      <c r="C87" s="46"/>
+      <c r="D87" s="46"/>
+      <c r="E87" s="46"/>
+      <c r="F87" s="46"/>
+      <c r="G87" s="46"/>
+      <c r="H87" s="46"/>
+      <c r="I87" s="46"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>114</v>
       </c>
-      <c r="B85" s="23">
+      <c r="B88" s="23">
         <f>0.5*B21*(B3/(B23*10^-6))*(1/B9)*2</f>
         <v>0.33812341504649202</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C88" t="s">
         <v>23</v>
       </c>
-      <c r="F85" s="47" t="s">
+      <c r="F88" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="G85" s="47"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+      <c r="G88" s="49"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>116</v>
       </c>
-      <c r="B86" s="23">
-        <f>B100</f>
+      <c r="B89" s="23">
+        <f>B106</f>
         <v>956.13236267372599</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D89" t="s">
         <v>117</v>
       </c>
-      <c r="F86" s="47"/>
-      <c r="G86" s="47"/>
-      <c r="H86" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>115</v>
-      </c>
-      <c r="B87" s="23">
+      <c r="F89" s="49"/>
+      <c r="G89" s="49"/>
+      <c r="H89" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>177</v>
+      </c>
+      <c r="B90" s="23">
         <f>(1/B21)*(B7+(B31/2))</f>
         <v>7.6039599999999998</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C90" t="s">
         <v>23</v>
       </c>
-      <c r="F87" s="47"/>
-      <c r="G87" s="47"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B88" s="23"/>
-      <c r="F88" s="44"/>
-      <c r="G88" s="44"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>74</v>
-      </c>
-      <c r="B89" s="23">
-        <v>2</v>
-      </c>
-      <c r="C89" t="s">
-        <v>42</v>
-      </c>
-      <c r="F89" s="44"/>
-      <c r="G89" s="44"/>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B90" s="23"/>
-      <c r="F90" s="44"/>
-      <c r="G90" s="44"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>120</v>
-      </c>
-      <c r="B91" s="4">
-        <f>B85^2*B89</f>
-        <v>0.22865488760540462</v>
-      </c>
-      <c r="C91" t="s">
-        <v>20</v>
-      </c>
+      <c r="F90" s="49"/>
+      <c r="G90" s="49"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B91" s="23"/>
       <c r="F91" s="44"/>
       <c r="G91" s="44"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>126</v>
-      </c>
-      <c r="B92" s="4" t="e">
-        <f>0.5*#REF!*D6*(#REF!/(1-B36))*(B89/2)*#REF!</f>
-        <v>#REF!</v>
+        <v>74</v>
+      </c>
+      <c r="B92" s="23">
+        <f>1*1.5</f>
+        <v>1.5</v>
       </c>
       <c r="C92" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="F92" s="44"/>
       <c r="G92" s="44"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>127</v>
-      </c>
-      <c r="B93" s="4" t="e">
-        <f>0.5*#REF!*D6*#REF!*(B89/2)*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C93" t="s">
-        <v>20</v>
-      </c>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B93" s="23"/>
       <c r="F93" s="44"/>
       <c r="G93" s="44"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>129</v>
-      </c>
-      <c r="B94" s="4" t="e">
-        <f>B91+#REF!+B92+B93</f>
-        <v>#REF!</v>
+        <v>120</v>
+      </c>
+      <c r="B94" s="4">
+        <f>B88^2*B92</f>
+        <v>0.17149116570405346</v>
       </c>
       <c r="C94" t="s">
         <v>20</v>
@@ -4551,644 +4561,839 @@
       <c r="F94" s="44"/>
       <c r="G94" s="44"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>179</v>
+      </c>
+      <c r="B95" s="4">
+        <v>2</v>
+      </c>
       <c r="F95" s="44"/>
       <c r="G95" s="44"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B96" s="23"/>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>178</v>
+      </c>
+      <c r="B96" s="4">
+        <f>B94*B95</f>
+        <v>0.34298233140810691</v>
+      </c>
+      <c r="C96" t="s">
+        <v>20</v>
+      </c>
       <c r="F96" s="44"/>
       <c r="G96" s="44"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B97" s="23"/>
-      <c r="F97" s="44"/>
-      <c r="G97" s="44"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B98" s="23"/>
-      <c r="F98" s="44"/>
-      <c r="G98" s="44"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99" s="45" t="s">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B97" s="4"/>
+      <c r="F97" s="45"/>
+      <c r="G97" s="45"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B98" s="22"/>
+      <c r="C98" s="20"/>
+      <c r="D98" s="27"/>
+      <c r="E98" s="47" t="s">
+        <v>168</v>
+      </c>
+      <c r="F98" s="47"/>
+      <c r="G98" s="45"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>159</v>
+      </c>
+      <c r="B99" s="22">
+        <f>(B14-B13)/B96</f>
+        <v>218.67015624999993</v>
+      </c>
+      <c r="C99" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D99" s="27"/>
+      <c r="E99" s="14">
+        <v>0.35</v>
+      </c>
+      <c r="F99" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="G99" s="45"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>162</v>
+      </c>
+      <c r="B100" s="25">
+        <v>0.6</v>
+      </c>
+      <c r="C100" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D100" s="27"/>
+      <c r="E100" s="20">
+        <f>E99*B102</f>
+        <v>21.91</v>
+      </c>
+      <c r="F100" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="G100" s="45"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>163</v>
+      </c>
+      <c r="B101" s="25">
+        <v>62</v>
+      </c>
+      <c r="C101" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D101" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="E101" s="20">
+        <f>1/E100</f>
+        <v>4.5641259698767686E-2</v>
+      </c>
+      <c r="F101" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="G101" s="45"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>180</v>
+      </c>
+      <c r="B102" s="22">
+        <f>B100+B101</f>
+        <v>62.6</v>
+      </c>
+      <c r="C102" s="20"/>
+      <c r="D102" s="27"/>
+      <c r="E102" s="20"/>
+      <c r="F102" s="20"/>
+      <c r="G102" s="44"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>181</v>
+      </c>
+      <c r="B103" s="22">
+        <f>(B96*B102)+B13</f>
+        <v>71.470693946147492</v>
+      </c>
+      <c r="C103" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="D103" s="27"/>
+      <c r="E103" s="20"/>
+      <c r="F103" s="20"/>
+      <c r="G103" s="44"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B104" s="22"/>
+      <c r="C104" s="20"/>
+      <c r="D104" s="27"/>
+      <c r="E104" s="20"/>
+      <c r="F104" s="20"/>
+      <c r="G104" s="44"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="B99" s="45"/>
-      <c r="C99" s="45"/>
-      <c r="D99" s="45"/>
-      <c r="E99" s="45"/>
-      <c r="F99" s="45"/>
-      <c r="G99" s="45"/>
-      <c r="H99" s="45"/>
-      <c r="I99" s="45"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+      <c r="B105" s="46"/>
+      <c r="C105" s="46"/>
+      <c r="D105" s="46"/>
+      <c r="E105" s="46"/>
+      <c r="F105" s="46"/>
+      <c r="G105" s="46"/>
+      <c r="H105" s="46"/>
+      <c r="I105" s="46"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>118</v>
       </c>
-      <c r="B100" s="4">
+      <c r="B106" s="4">
         <f>((B6^2)/(B6-(B3*B21)))*1.2</f>
         <v>956.13236267372599</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C106" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>119</v>
       </c>
-      <c r="B101" s="4">
-        <f>SQRT(B106/B102)</f>
+      <c r="B107" s="4">
+        <f>SQRT(B112/B108)</f>
         <v>5.5123576586177476</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C107" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>74</v>
       </c>
-      <c r="B102">
-        <v>0.2</v>
-      </c>
-      <c r="C102" t="s">
+      <c r="B108">
+        <f>0.15*1.5</f>
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="C108" t="s">
         <v>42</v>
       </c>
-      <c r="F102" s="47" t="s">
+      <c r="F108" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="G102" s="47"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
+      <c r="G108" s="49"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>122</v>
       </c>
-      <c r="B103" s="1">
-        <f>D103*10^-9</f>
+      <c r="B109" s="1">
+        <f>D109*10^-9</f>
         <v>3.0000000000000004E-8</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C109" t="s">
         <v>125</v>
       </c>
-      <c r="D103" s="14">
+      <c r="D109" s="14">
         <v>30</v>
       </c>
-      <c r="E103" t="s">
+      <c r="E109" t="s">
         <v>124</v>
       </c>
-      <c r="F103" s="47"/>
-      <c r="G103" s="47"/>
-      <c r="H103" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
+      <c r="F109" s="49"/>
+      <c r="G109" s="49"/>
+      <c r="H109" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>128</v>
       </c>
-      <c r="B104" s="1">
-        <f>D104*10^-9</f>
+      <c r="B110" s="1">
+        <f>D110*10^-9</f>
         <v>6.0000000000000008E-9</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C110" t="s">
         <v>125</v>
       </c>
-      <c r="D104">
+      <c r="D110">
         <v>6</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E110" t="s">
         <v>124</v>
       </c>
-      <c r="F104" s="47"/>
-      <c r="G104" s="47"/>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
+      <c r="F110" s="49"/>
+      <c r="G110" s="49"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>120</v>
       </c>
-      <c r="B106" s="4">
-        <f>B21*(B3/B5)*((1/B21)*B7)^2*B102</f>
-        <v>6.0772173913043472</v>
-      </c>
-      <c r="C106" t="s">
+      <c r="B112" s="4">
+        <f>B21*(B3/B5)*((1/B21)*B7)^2*B108</f>
+        <v>6.8368695652173894</v>
+      </c>
+      <c r="C112" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>121</v>
       </c>
-      <c r="B107">
-        <f>B103*B11*B9</f>
+      <c r="B113">
+        <f>B109*B11*B9</f>
         <v>3.0000000000000002E-2</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C113" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>126</v>
       </c>
-      <c r="B108" s="4">
-        <f>0.5*B7*D21*(B6/(1-B51))*(B104/2)*B9</f>
+      <c r="B114" s="4">
+        <f>0.5*B7*D21*(B6/(1-B51))*(B110/2)*B9</f>
         <v>1.6124303247480403</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C114" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>127</v>
       </c>
-      <c r="B109" s="4">
-        <f>0.5*B7*D21*B6*(B104/2)*B9</f>
+      <c r="B115" s="4">
+        <f>0.5*B7*D21*B6*(B110/2)*B9</f>
         <v>0.68796000000000002</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C115" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>129</v>
       </c>
-      <c r="B110" s="4">
-        <f>B106+B107+B108+B109</f>
-        <v>8.4076077160523877</v>
-      </c>
-      <c r="C110" t="s">
+      <c r="B116" s="4">
+        <f>B112+B113+B114+B115</f>
+        <v>9.1672598899654307</v>
+      </c>
+      <c r="C116" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B111" s="4"/>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B112" s="22"/>
-      <c r="C112" s="20"/>
-      <c r="D112" s="27"/>
-      <c r="E112" s="48" t="s">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B117" s="4"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B118" s="22"/>
+      <c r="C118" s="20"/>
+      <c r="D118" s="27"/>
+      <c r="E118" s="47" t="s">
         <v>168</v>
       </c>
-      <c r="F112" s="48"/>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
+      <c r="F118" s="47"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>159</v>
       </c>
-      <c r="B113" s="22">
-        <f>(B14-B13)/B110</f>
-        <v>8.9204923127900937</v>
-      </c>
-      <c r="C113" s="20" t="s">
+      <c r="B119" s="22">
+        <f>(B14-B13)/B116</f>
+        <v>8.1812887275177726</v>
+      </c>
+      <c r="C119" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="D113" s="27"/>
-      <c r="E113" s="14">
+      <c r="D119" s="27"/>
+      <c r="E119" s="14">
         <v>0.35</v>
       </c>
-      <c r="F113" s="20" t="s">
+      <c r="F119" s="20" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>162</v>
       </c>
-      <c r="B114" s="25">
+      <c r="B120" s="25">
         <v>0.9</v>
       </c>
-      <c r="C114" s="20" t="s">
+      <c r="C120" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="D114" s="27"/>
-      <c r="E114" s="20">
-        <f>E113*B116</f>
+      <c r="D120" s="27"/>
+      <c r="E120" s="20">
+        <f>E119*B122</f>
         <v>112.84</v>
       </c>
-      <c r="F114" s="20" t="s">
+      <c r="F120" s="20" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>163</v>
       </c>
-      <c r="B115" s="25">
+      <c r="B121" s="25">
         <v>1</v>
       </c>
-      <c r="C115" s="20" t="s">
+      <c r="C121" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="D115" s="27" t="s">
-        <v>172</v>
-      </c>
-      <c r="E115" s="20">
-        <f>1/E114</f>
+      <c r="D121" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="E121" s="20">
+        <f>1/E120</f>
         <v>8.8621056362991838E-3</v>
       </c>
-      <c r="F115" s="20" t="s">
+      <c r="F121" s="20" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>164</v>
       </c>
-      <c r="B116" s="22">
+      <c r="B122" s="22">
         <f>15.5*20.8</f>
         <v>322.40000000000003</v>
       </c>
-      <c r="C116" s="20" t="s">
+      <c r="C122" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="D116" s="27"/>
-      <c r="E116" s="20"/>
-      <c r="F116" s="20"/>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
+      <c r="D122" s="27"/>
+      <c r="E122" s="20"/>
+      <c r="F122" s="20"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>166</v>
       </c>
-      <c r="B117" s="22">
-        <f>E115</f>
+      <c r="B123" s="22">
+        <f>E121</f>
         <v>8.8621056362991838E-3</v>
       </c>
-      <c r="C117" s="20" t="s">
+      <c r="C123" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="D117" s="27"/>
-      <c r="E117" s="20"/>
-      <c r="F117" s="20"/>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
+      <c r="D123" s="27"/>
+      <c r="E123" s="20"/>
+      <c r="F123" s="20"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>167</v>
       </c>
-      <c r="B118" s="22">
-        <f>B113-B114-B115-B117</f>
-        <v>7.0116302071537939</v>
-      </c>
-      <c r="C118" s="20" t="s">
+      <c r="B124" s="22">
+        <f>B119-B120-B121-B123</f>
+        <v>6.2724266218814728</v>
+      </c>
+      <c r="C124" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="D118" s="27"/>
-      <c r="E118" s="20"/>
-      <c r="F118" s="20"/>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B119" s="22"/>
-      <c r="C119" s="20"/>
-      <c r="D119" s="27"/>
-      <c r="E119" s="20"/>
-      <c r="F119" s="20"/>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
-        <v>174</v>
-      </c>
-      <c r="B120">
+      <c r="D124" s="27"/>
+      <c r="E124" s="20"/>
+      <c r="F124" s="20"/>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B125" s="22"/>
+      <c r="C125" s="20"/>
+      <c r="D125" s="27"/>
+      <c r="E125" s="20"/>
+      <c r="F125" s="20"/>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>173</v>
+      </c>
+      <c r="B126">
         <v>3.9</v>
       </c>
-      <c r="C120" s="20" t="s">
+      <c r="C126" s="20" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A121" s="45" t="s">
+      <c r="D126" s="27"/>
+      <c r="E126" s="20"/>
+      <c r="F126" s="20"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>180</v>
+      </c>
+      <c r="B127" s="21">
+        <f>B120+B121+B123+B126</f>
+        <v>5.8088621056362992</v>
+      </c>
+      <c r="C127" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D127" s="27"/>
+      <c r="E127" s="20"/>
+      <c r="F127" s="20"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C128" s="20"/>
+      <c r="D128" s="27"/>
+      <c r="E128" s="20"/>
+      <c r="F128" s="20"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>181</v>
+      </c>
+      <c r="B129">
+        <f>B13+B116*B127</f>
+        <v>103.25134858733978</v>
+      </c>
+      <c r="C129" s="20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="B121" s="45"/>
-      <c r="C121" s="45"/>
-      <c r="D121" s="45"/>
-      <c r="E121" s="45"/>
-      <c r="F121" s="45"/>
-      <c r="G121" s="45"/>
-      <c r="H121" s="45"/>
-      <c r="I121" s="45"/>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
+      <c r="B130" s="46"/>
+      <c r="C130" s="46"/>
+      <c r="D130" s="46"/>
+      <c r="E130" s="46"/>
+      <c r="F130" s="46"/>
+      <c r="G130" s="46"/>
+      <c r="H130" s="46"/>
+      <c r="I130" s="46"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>135</v>
       </c>
-      <c r="B122" s="4">
+      <c r="B131" s="4">
         <f>(B3/(1-(B3/(B5*D21))))*1.2</f>
         <v>67.501007838745792</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C131" t="s">
         <v>10</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D131" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>135</v>
       </c>
-      <c r="B123" s="4">
+      <c r="B132" s="4">
         <f>(B3/(B9*2*SQRT(B23*10^-6*B49)))</f>
         <v>30.154861431004125</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C132" t="s">
         <v>10</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D132" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>138</v>
       </c>
-      <c r="B124">
+      <c r="B133">
         <f>SQRT(B51*(B7^2+(B31^2/12)))</f>
         <v>30.297673990121055</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C133" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F125" s="47" t="s">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F134" s="49" t="s">
         <v>141</v>
       </c>
-      <c r="G125" s="47"/>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
+      <c r="G134" s="49"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>74</v>
       </c>
-      <c r="B126" s="21">
-        <f>D126*10^-3</f>
-        <v>1.9E-3</v>
-      </c>
-      <c r="C126" t="s">
+      <c r="B135" s="21">
+        <f>D135*10^-3</f>
+        <v>2.0400000000000001E-3</v>
+      </c>
+      <c r="C135" t="s">
         <v>42</v>
       </c>
-      <c r="D126">
-        <v>1.9</v>
-      </c>
-      <c r="E126" t="s">
+      <c r="D135">
+        <f>1.7*1.2</f>
+        <v>2.04</v>
+      </c>
+      <c r="E135" t="s">
         <v>43</v>
       </c>
-      <c r="F126" s="47"/>
-      <c r="G126" s="47"/>
-      <c r="H126" t="s">
+      <c r="F135" s="49"/>
+      <c r="G135" s="49"/>
+      <c r="H135" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>122</v>
+      </c>
+      <c r="B136" s="1">
+        <f>D136*10^-9</f>
+        <v>1.24E-7</v>
+      </c>
+      <c r="C136" t="s">
+        <v>125</v>
+      </c>
+      <c r="D136">
+        <v>124</v>
+      </c>
+      <c r="E136" t="s">
+        <v>124</v>
+      </c>
+      <c r="F136" s="49"/>
+      <c r="G136" s="49"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>139</v>
+      </c>
+      <c r="B138" s="4">
+        <f>(B133^2*B135)+(B11*B136*B9)</f>
+        <v>1.9966160603917822</v>
+      </c>
+      <c r="C138" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B139" s="4"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B140" s="22"/>
+      <c r="C140" s="20"/>
+      <c r="D140" s="27"/>
+      <c r="E140" s="47" t="s">
+        <v>168</v>
+      </c>
+      <c r="F140" s="47"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>159</v>
+      </c>
+      <c r="B141" s="22">
+        <f>(B14-B13)/B138</f>
+        <v>37.563556403169102</v>
+      </c>
+      <c r="C141" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D141" s="27"/>
+      <c r="E141" s="14">
+        <v>0.35</v>
+      </c>
+      <c r="F141" s="20" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>162</v>
+      </c>
+      <c r="B142" s="25">
+        <v>0.6</v>
+      </c>
+      <c r="C142" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D142" s="27"/>
+      <c r="E142" s="20">
+        <f>E141*B144</f>
+        <v>59.005099999999999</v>
+      </c>
+      <c r="F142" s="20" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>163</v>
+      </c>
+      <c r="B143" s="25">
+        <v>1</v>
+      </c>
+      <c r="C143" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D143" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="E143" s="20">
+        <f>1/E142</f>
+        <v>1.6947687572769134E-2</v>
+      </c>
+      <c r="F143" s="20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>164</v>
+      </c>
+      <c r="B144" s="22">
+        <f>10.67*15.8</f>
+        <v>168.58600000000001</v>
+      </c>
+      <c r="C144" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="D144" s="27"/>
+      <c r="E144" s="20"/>
+      <c r="F144" s="20"/>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>166</v>
+      </c>
+      <c r="B145" s="22">
+        <f>E143</f>
+        <v>1.6947687572769134E-2</v>
+      </c>
+      <c r="C145" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D145" s="27"/>
+      <c r="E145" s="20"/>
+      <c r="F145" s="20"/>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>167</v>
+      </c>
+      <c r="B146" s="22">
+        <f>B141-B142-B143-B145</f>
+        <v>35.946608715596334</v>
+      </c>
+      <c r="C146" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D146" s="27"/>
+      <c r="E146" s="20"/>
+      <c r="F146" s="20"/>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B147" s="22"/>
+      <c r="C147" s="20"/>
+      <c r="D147" s="27"/>
+      <c r="E147" s="20"/>
+      <c r="F147" s="20"/>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
-        <v>122</v>
-      </c>
-      <c r="B127" s="1">
-        <f>D127*10^-9</f>
-        <v>1.24E-7</v>
-      </c>
-      <c r="C127" t="s">
-        <v>125</v>
-      </c>
-      <c r="D127">
-        <v>124</v>
-      </c>
-      <c r="E127" t="s">
-        <v>124</v>
-      </c>
-      <c r="F127" s="47"/>
-      <c r="G127" s="47"/>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
-        <v>139</v>
-      </c>
-      <c r="B129" s="4">
-        <f>(B124^2*B126)+(B11*B127*B9)</f>
-        <v>1.8681031935021499</v>
-      </c>
-      <c r="C129" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B130" s="4"/>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B131" s="22"/>
-      <c r="C131" s="20"/>
-      <c r="D131" s="27"/>
-      <c r="E131" s="48" t="s">
-        <v>168</v>
-      </c>
-      <c r="F131" s="48"/>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>159</v>
-      </c>
-      <c r="B132" s="22">
-        <f>(B14-B13)/B129</f>
-        <v>40.147675064671787</v>
-      </c>
-      <c r="C132" s="20" t="s">
+      <c r="B148">
+        <v>12</v>
+      </c>
+      <c r="C148" t="s">
         <v>161</v>
       </c>
-      <c r="D132" s="27"/>
-      <c r="E132" s="14">
-        <v>0.35</v>
-      </c>
-      <c r="F132" s="20" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
-        <v>162</v>
-      </c>
-      <c r="B133" s="25">
-        <v>0.6</v>
-      </c>
-      <c r="C133" s="20" t="s">
+      <c r="D148" s="27"/>
+      <c r="E148" s="20"/>
+      <c r="F148" s="20"/>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>180</v>
+      </c>
+      <c r="B149" s="21">
+        <f>B142+B143+B145+B148</f>
+        <v>13.61694768757277</v>
+      </c>
+      <c r="C149" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="D133" s="27"/>
-      <c r="E133" s="20">
-        <f>E132*B135</f>
-        <v>112.84</v>
-      </c>
-      <c r="F133" s="20" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
-        <v>163</v>
-      </c>
-      <c r="B134" s="25">
-        <v>1</v>
-      </c>
-      <c r="C134" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="D134" s="27" t="s">
-        <v>172</v>
-      </c>
-      <c r="E134" s="20">
-        <f>1/E133</f>
-        <v>8.8621056362991838E-3</v>
-      </c>
-      <c r="F134" s="20" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
-        <v>164</v>
-      </c>
-      <c r="B135" s="22">
-        <f>15.5*20.8</f>
-        <v>322.40000000000003</v>
-      </c>
-      <c r="C135" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="D135" s="27"/>
-      <c r="E135" s="20"/>
-      <c r="F135" s="20"/>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
-        <v>166</v>
-      </c>
-      <c r="B136" s="22">
-        <f>E134</f>
-        <v>8.8621056362991838E-3</v>
-      </c>
-      <c r="C136" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="D136" s="27"/>
-      <c r="E136" s="20"/>
-      <c r="F136" s="20"/>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
-        <v>167</v>
-      </c>
-      <c r="B137" s="22">
-        <f>B132-B133-B134-B136</f>
-        <v>38.538812959035489</v>
-      </c>
-      <c r="C137" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="D137" s="27"/>
-      <c r="E137" s="20"/>
-      <c r="F137" s="20"/>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B138" s="22"/>
-      <c r="C138" s="20"/>
-      <c r="D138" s="27"/>
-      <c r="E138" s="20"/>
-      <c r="F138" s="20"/>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A139" t="s">
-        <v>177</v>
-      </c>
-      <c r="B139">
-        <v>12</v>
-      </c>
-      <c r="C139" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A140" s="45" t="s">
+      <c r="D149" s="27"/>
+      <c r="E149" s="20"/>
+      <c r="F149" s="20"/>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C150" s="20"/>
+      <c r="D150" s="27"/>
+      <c r="E150" s="20"/>
+      <c r="F150" s="20"/>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>181</v>
+      </c>
+      <c r="B151">
+        <f>B13+B138*B149</f>
+        <v>77.187816446522532</v>
+      </c>
+      <c r="C151" s="20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A152" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="B140" s="45"/>
-      <c r="C140" s="45"/>
-      <c r="D140" s="45"/>
-      <c r="E140" s="45"/>
-      <c r="F140" s="45"/>
-      <c r="G140" s="45"/>
-      <c r="H140" s="45"/>
-      <c r="I140" s="45"/>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A141" t="s">
+      <c r="B152" s="46"/>
+      <c r="C152" s="46"/>
+      <c r="D152" s="46"/>
+      <c r="E152" s="46"/>
+      <c r="F152" s="46"/>
+      <c r="G152" s="46"/>
+      <c r="H152" s="46"/>
+      <c r="I152" s="46"/>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A142" t="s">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>151</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B154" t="s">
         <v>146</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C154" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>147</v>
       </c>
-      <c r="B143">
+      <c r="B155">
         <v>15</v>
       </c>
-      <c r="C143">
+      <c r="C155">
         <v>6.25</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
         <v>150</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B156" t="s">
         <v>148</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C156" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>149</v>
       </c>
-      <c r="B145">
+      <c r="B157">
         <v>800</v>
       </c>
-      <c r="C145">
+      <c r="C157">
         <v>1000</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A140:I140"/>
+  <mergeCells count="17">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="G63:I66"/>
+    <mergeCell ref="A130:I130"/>
+    <mergeCell ref="F134:G136"/>
+    <mergeCell ref="A87:I87"/>
+    <mergeCell ref="A105:I105"/>
+    <mergeCell ref="F108:G110"/>
+    <mergeCell ref="F88:G90"/>
+    <mergeCell ref="E98:F98"/>
+    <mergeCell ref="A152:I152"/>
     <mergeCell ref="A47:I47"/>
     <mergeCell ref="A15:I15"/>
     <mergeCell ref="A29:I29"/>
     <mergeCell ref="A56:I56"/>
     <mergeCell ref="E75:F75"/>
-    <mergeCell ref="E112:F112"/>
-    <mergeCell ref="E131:F131"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="G63:I66"/>
-    <mergeCell ref="A121:I121"/>
-    <mergeCell ref="F125:G127"/>
-    <mergeCell ref="A84:I84"/>
-    <mergeCell ref="A99:I99"/>
-    <mergeCell ref="F102:G104"/>
-    <mergeCell ref="F85:G87"/>
+    <mergeCell ref="E118:F118"/>
+    <mergeCell ref="E140:F140"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -5208,27 +5413,27 @@
       <selection activeCell="O22" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="16" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="21" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.5546875" style="36"/>
+    <col min="11" max="16" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="21" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.5703125" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A1" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-    </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5236,7 +5441,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -5250,7 +5455,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -5261,7 +5466,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -5275,7 +5480,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -5289,7 +5494,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -5301,7 +5506,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -5412,7 +5617,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -5423,7 +5628,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -5434,23 +5639,23 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="B12" s="20"/>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A13" s="45" t="s">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A13" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-    </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="B13" s="46"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -5467,7 +5672,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -5478,7 +5683,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -5494,7 +5699,7 @@
         <v>6.708333333333333</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -5503,7 +5708,7 @@
         <v>10.989010989010989</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -5522,7 +5727,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>18</v>
       </c>
@@ -5533,7 +5738,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -5564,7 +5769,7 @@
         <v>10.989010989010989</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -5591,7 +5796,7 @@
         <v>3900</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>35</v>
       </c>
@@ -5608,7 +5813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -5619,7 +5824,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -5628,20 +5833,20 @@
         <v>0.99923076923076926</v>
       </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A27" s="45" t="s">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A27" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="B27" s="45"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="45"/>
-    </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="B27" s="46"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+    </row>
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -5653,7 +5858,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -5665,7 +5870,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -5811,7 +6016,7 @@
         <v>1.599976110845676</v>
       </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -5957,7 +6162,7 @@
         <v>2.9650706436420724</v>
       </c>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:41" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>25</v>
       </c>
@@ -5977,10 +6182,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:41" ht="15.75" x14ac:dyDescent="0.3">
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:41" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -5998,7 +6203,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:41" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -6007,7 +6212,7 @@
       </c>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:41" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -6156,7 +6361,7 @@
         <v>-1.6891891891891893</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -6175,7 +6380,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -6193,7 +6398,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -6205,7 +6410,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -6217,7 +6422,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -6239,7 +6444,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -6386,20 +6591,20 @@
         <v>37.003448275862688</v>
       </c>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A45" s="45" t="s">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A45" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-    </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="B45" s="46"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="46"/>
+      <c r="H45" s="46"/>
+      <c r="I45" s="46"/>
+    </row>
+    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -6410,7 +6615,7 @@
       <c r="G46" s="20"/>
       <c r="H46" s="20"/>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -6558,7 +6763,7 @@
         <v>0.25378340977707292</v>
       </c>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -6704,7 +6909,7 @@
         <v>1.5227004586624375</v>
       </c>
     </row>
-    <row r="49" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -6713,7 +6918,7 @@
         <v>0.5733397037744864</v>
       </c>
     </row>
-    <row r="50" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -6852,7 +7057,7 @@
         <v>9187.9465249293535</v>
       </c>
     </row>
-    <row r="52" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>71</v>
       </c>
@@ -6897,20 +7102,20 @@
       <c r="AO52" s="42"/>
       <c r="AP52" s="20"/>
     </row>
-    <row r="54" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A54" s="45" t="s">
+    <row r="54" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A54" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="B54" s="45"/>
-      <c r="C54" s="45"/>
-      <c r="D54" s="45"/>
-      <c r="E54" s="45"/>
-      <c r="F54" s="45"/>
-      <c r="G54" s="45"/>
-      <c r="H54" s="45"/>
-      <c r="I54" s="45"/>
-    </row>
-    <row r="55" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="B54" s="46"/>
+      <c r="C54" s="46"/>
+      <c r="D54" s="46"/>
+      <c r="E54" s="46"/>
+      <c r="F54" s="46"/>
+      <c r="G54" s="46"/>
+      <c r="H54" s="46"/>
+      <c r="I54" s="46"/>
+    </row>
+    <row r="55" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>81</v>
       </c>
@@ -6925,7 +7130,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>73</v>
       </c>
@@ -6939,7 +7144,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>74</v>
       </c>
@@ -6957,7 +7162,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="59" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>72</v>
       </c>
@@ -6982,7 +7187,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>87</v>
       </c>
@@ -6994,14 +7199,14 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="G61" s="46" t="s">
+    <row r="61" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="G61" s="48" t="s">
         <v>143</v>
       </c>
-      <c r="H61" s="47"/>
-      <c r="I61" s="47"/>
-    </row>
-    <row r="62" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="H61" s="49"/>
+      <c r="I61" s="49"/>
+    </row>
+    <row r="62" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>77</v>
       </c>
@@ -7011,11 +7216,11 @@
       <c r="C62" t="s">
         <v>79</v>
       </c>
-      <c r="G62" s="47"/>
-      <c r="H62" s="47"/>
-      <c r="I62" s="47"/>
-    </row>
-    <row r="63" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="G62" s="49"/>
+      <c r="H62" s="49"/>
+      <c r="I62" s="49"/>
+    </row>
+    <row r="63" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>78</v>
       </c>
@@ -7025,11 +7230,11 @@
       <c r="C63" t="s">
         <v>10</v>
       </c>
-      <c r="G63" s="47"/>
-      <c r="H63" s="47"/>
-      <c r="I63" s="47"/>
-    </row>
-    <row r="64" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="G63" s="49"/>
+      <c r="H63" s="49"/>
+      <c r="I63" s="49"/>
+    </row>
+    <row r="64" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>76</v>
       </c>
@@ -7047,11 +7252,11 @@
       <c r="E64" t="s">
         <v>75</v>
       </c>
-      <c r="G64" s="47"/>
-      <c r="H64" s="47"/>
-      <c r="I64" s="47"/>
-    </row>
-    <row r="65" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="G64" s="49"/>
+      <c r="H64" s="49"/>
+      <c r="I64" s="49"/>
+    </row>
+    <row r="65" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>89</v>
       </c>
@@ -7072,7 +7277,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="67" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>80</v>
       </c>
@@ -7086,7 +7291,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="68" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>84</v>
       </c>
@@ -7114,12 +7319,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:41" x14ac:dyDescent="0.25">
       <c r="D69" s="27"/>
       <c r="E69" s="20"/>
       <c r="F69" s="20"/>
     </row>
-    <row r="70" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>138</v>
       </c>
@@ -7134,7 +7339,7 @@
       <c r="E70" s="20"/>
       <c r="F70" s="20"/>
     </row>
-    <row r="71" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>122</v>
       </c>
@@ -7153,7 +7358,7 @@
       </c>
       <c r="F71" s="20"/>
     </row>
-    <row r="72" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>140</v>
       </c>
@@ -7295,20 +7500,20 @@
         <v>6.6360555381126796</v>
       </c>
     </row>
-    <row r="74" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A74" s="45" t="s">
+    <row r="74" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A74" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="B74" s="45"/>
-      <c r="C74" s="45"/>
-      <c r="D74" s="45"/>
-      <c r="E74" s="45"/>
-      <c r="F74" s="45"/>
-      <c r="G74" s="45"/>
-      <c r="H74" s="45"/>
-      <c r="I74" s="45"/>
-    </row>
-    <row r="75" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="B74" s="46"/>
+      <c r="C74" s="46"/>
+      <c r="D74" s="46"/>
+      <c r="E74" s="46"/>
+      <c r="F74" s="46"/>
+      <c r="G74" s="46"/>
+      <c r="H74" s="46"/>
+      <c r="I74" s="46"/>
+    </row>
+    <row r="75" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>114</v>
       </c>
@@ -7319,10 +7524,10 @@
       <c r="C75" t="s">
         <v>23</v>
       </c>
-      <c r="F75" s="47" t="s">
+      <c r="F75" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="G75" s="47"/>
+      <c r="G75" s="49"/>
       <c r="J75" t="s">
         <v>23</v>
       </c>
@@ -7451,7 +7656,7 @@
         <v>8.4530853761623004E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>116</v>
       </c>
@@ -7462,10 +7667,10 @@
       <c r="D76" t="s">
         <v>117</v>
       </c>
-      <c r="F76" s="47"/>
-      <c r="G76" s="47"/>
-    </row>
-    <row r="77" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="F76" s="49"/>
+      <c r="G76" s="49"/>
+    </row>
+    <row r="77" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>115</v>
       </c>
@@ -7476,23 +7681,23 @@
       <c r="C77" t="s">
         <v>23</v>
       </c>
-      <c r="F77" s="47"/>
-      <c r="G77" s="47"/>
-    </row>
-    <row r="78" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A78" s="45" t="s">
+      <c r="F77" s="49"/>
+      <c r="G77" s="49"/>
+    </row>
+    <row r="78" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A78" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="B78" s="45"/>
-      <c r="C78" s="45"/>
-      <c r="D78" s="45"/>
-      <c r="E78" s="45"/>
-      <c r="F78" s="45"/>
-      <c r="G78" s="45"/>
-      <c r="H78" s="45"/>
-      <c r="I78" s="45"/>
-    </row>
-    <row r="79" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="B78" s="46"/>
+      <c r="C78" s="46"/>
+      <c r="D78" s="46"/>
+      <c r="E78" s="46"/>
+      <c r="F78" s="46"/>
+      <c r="G78" s="46"/>
+      <c r="H78" s="46"/>
+      <c r="I78" s="46"/>
+    </row>
+    <row r="79" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>118</v>
       </c>
@@ -7504,7 +7709,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>119</v>
       </c>
@@ -7516,7 +7721,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>74</v>
       </c>
@@ -7526,12 +7731,12 @@
       <c r="C81" t="s">
         <v>42</v>
       </c>
-      <c r="F81" s="47" t="s">
+      <c r="F81" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="G81" s="47"/>
-    </row>
-    <row r="82" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="G81" s="49"/>
+    </row>
+    <row r="82" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>122</v>
       </c>
@@ -7548,10 +7753,10 @@
       <c r="E82" t="s">
         <v>124</v>
       </c>
-      <c r="F82" s="47"/>
-      <c r="G82" s="47"/>
-    </row>
-    <row r="83" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="F82" s="49"/>
+      <c r="G82" s="49"/>
+    </row>
+    <row r="83" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>128</v>
       </c>
@@ -7568,10 +7773,10 @@
       <c r="E83" t="s">
         <v>124</v>
       </c>
-      <c r="F83" s="47"/>
-      <c r="G83" s="47"/>
-    </row>
-    <row r="85" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="F83" s="49"/>
+      <c r="G83" s="49"/>
+    </row>
+    <row r="85" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>120</v>
       </c>
@@ -7583,7 +7788,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>121</v>
       </c>
@@ -7719,7 +7924,7 @@
         <v>0.12000000000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>126</v>
       </c>
@@ -7855,7 +8060,7 @@
         <v>6.4497212989921611</v>
       </c>
     </row>
-    <row r="88" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>127</v>
       </c>
@@ -7991,7 +8196,7 @@
         <v>2.7518400000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>129</v>
       </c>
@@ -8127,20 +8332,20 @@
         <v>15.398778690296508</v>
       </c>
     </row>
-    <row r="90" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A90" s="45" t="s">
+    <row r="90" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A90" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="B90" s="45"/>
-      <c r="C90" s="45"/>
-      <c r="D90" s="45"/>
-      <c r="E90" s="45"/>
-      <c r="F90" s="45"/>
-      <c r="G90" s="45"/>
-      <c r="H90" s="45"/>
-      <c r="I90" s="45"/>
-    </row>
-    <row r="91" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="B90" s="46"/>
+      <c r="C90" s="46"/>
+      <c r="D90" s="46"/>
+      <c r="E90" s="46"/>
+      <c r="F90" s="46"/>
+      <c r="G90" s="46"/>
+      <c r="H90" s="46"/>
+      <c r="I90" s="46"/>
+    </row>
+    <row r="91" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>135</v>
       </c>
@@ -8155,7 +8360,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="92" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>135</v>
       </c>
@@ -8297,7 +8502,7 @@
         <v>30.154861431004125</v>
       </c>
     </row>
-    <row r="93" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>138</v>
       </c>
@@ -8309,13 +8514,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="F94" s="47" t="s">
+    <row r="94" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="F94" s="49" t="s">
         <v>141</v>
       </c>
-      <c r="G94" s="47"/>
-    </row>
-    <row r="95" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="G94" s="49"/>
+    </row>
+    <row r="95" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>74</v>
       </c>
@@ -8332,10 +8537,10 @@
       <c r="E95" t="s">
         <v>43</v>
       </c>
-      <c r="F95" s="47"/>
-      <c r="G95" s="47"/>
-    </row>
-    <row r="96" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="F95" s="49"/>
+      <c r="G95" s="49"/>
+    </row>
+    <row r="96" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>122</v>
       </c>
@@ -8352,10 +8557,10 @@
       <c r="E96" t="s">
         <v>124</v>
       </c>
-      <c r="F96" s="47"/>
-      <c r="G96" s="47"/>
-    </row>
-    <row r="98" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="F96" s="49"/>
+      <c r="G96" s="49"/>
+    </row>
+    <row r="98" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>139</v>
       </c>
@@ -8494,25 +8699,25 @@
         <v>2.2621920688007644</v>
       </c>
     </row>
-    <row r="100" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A100" s="45" t="s">
+    <row r="100" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A100" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="B100" s="45"/>
-      <c r="C100" s="45"/>
-      <c r="D100" s="45"/>
-      <c r="E100" s="45"/>
-      <c r="F100" s="45"/>
-      <c r="G100" s="45"/>
-      <c r="H100" s="45"/>
-      <c r="I100" s="45"/>
-    </row>
-    <row r="101" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="B100" s="46"/>
+      <c r="C100" s="46"/>
+      <c r="D100" s="46"/>
+      <c r="E100" s="46"/>
+      <c r="F100" s="46"/>
+      <c r="G100" s="46"/>
+      <c r="H100" s="46"/>
+      <c r="I100" s="46"/>
+    </row>
+    <row r="101" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="102" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>151</v>
       </c>
@@ -8523,7 +8728,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="103" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>147</v>
       </c>
@@ -8534,7 +8739,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="104" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>150</v>
       </c>
@@ -8545,7 +8750,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="105" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>149</v>
       </c>
@@ -8556,7 +8761,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="106" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:41" x14ac:dyDescent="0.25">
       <c r="I106" t="s">
         <v>154</v>
       </c>
@@ -8690,6 +8895,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="G61:I64"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A13:I13"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A45:I45"/>
+    <mergeCell ref="A54:I54"/>
     <mergeCell ref="A100:I100"/>
     <mergeCell ref="A74:I74"/>
     <mergeCell ref="F75:G77"/>
@@ -8697,12 +8908,6 @@
     <mergeCell ref="F81:G83"/>
     <mergeCell ref="A90:I90"/>
     <mergeCell ref="F94:G96"/>
-    <mergeCell ref="G61:I64"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A13:I13"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A45:I45"/>
-    <mergeCell ref="A54:I54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
worked on mosfet cooler calc
</commit_message>
<xml_diff>
--- a/DC_Converter_Calc.xlsx
+++ b/DC_Converter_Calc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Technik\Technik 2022\05 - Electronics\02 - HV\01 - HV Accumulator\02 - ECAD\02 - PCB Files\03 - HV_DCDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB66EDD-EFD3-4C51-BDBE-4BCD818C69D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF2F90A-1AF4-4BD7-A22C-68897CD83086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -733,14 +733,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3156,7 +3156,7 @@
   <dimension ref="A1:X157"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A62" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O80" sqref="O80"/>
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4046,11 +4046,11 @@
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="G63" s="48" t="s">
+      <c r="G63" s="47" t="s">
         <v>143</v>
       </c>
-      <c r="H63" s="49"/>
-      <c r="I63" s="49"/>
+      <c r="H63" s="48"/>
+      <c r="I63" s="48"/>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
@@ -4062,9 +4062,9 @@
       <c r="C64" t="s">
         <v>79</v>
       </c>
-      <c r="G64" s="49"/>
-      <c r="H64" s="49"/>
-      <c r="I64" s="49"/>
+      <c r="G64" s="48"/>
+      <c r="H64" s="48"/>
+      <c r="I64" s="48"/>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
@@ -4076,9 +4076,9 @@
       <c r="C65" t="s">
         <v>10</v>
       </c>
-      <c r="G65" s="49"/>
-      <c r="H65" s="49"/>
-      <c r="I65" s="49"/>
+      <c r="G65" s="48"/>
+      <c r="H65" s="48"/>
+      <c r="I65" s="48"/>
       <c r="J65" t="s">
         <v>174</v>
       </c>
@@ -4119,9 +4119,9 @@
       <c r="E66" t="s">
         <v>75</v>
       </c>
-      <c r="G66" s="49"/>
-      <c r="H66" s="49"/>
-      <c r="I66" s="49"/>
+      <c r="G66" s="48"/>
+      <c r="H66" s="48"/>
+      <c r="I66" s="48"/>
       <c r="R66" t="s">
         <v>94</v>
       </c>
@@ -4304,10 +4304,10 @@
       <c r="B75" s="22"/>
       <c r="C75" s="20"/>
       <c r="D75" s="27"/>
-      <c r="E75" s="47" t="s">
+      <c r="E75" s="49" t="s">
         <v>168</v>
       </c>
-      <c r="F75" s="47"/>
+      <c r="F75" s="49"/>
     </row>
     <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
@@ -4423,7 +4423,7 @@
         <v>182</v>
       </c>
       <c r="B83">
-        <v>4.2</v>
+        <v>4.7</v>
       </c>
       <c r="C83" s="20" t="s">
         <v>161</v>
@@ -4438,7 +4438,7 @@
       </c>
       <c r="B84" s="21">
         <f>B77+B78+B80+B83</f>
-        <v>4.455643293087248</v>
+        <v>4.955643293087248</v>
       </c>
       <c r="C84" s="20"/>
       <c r="D84" s="27"/>
@@ -4457,7 +4457,7 @@
       </c>
       <c r="B86">
         <f>B13+B74*B84</f>
-        <v>96.661523963891455</v>
+        <v>101.89775147297919</v>
       </c>
       <c r="C86" t="s">
         <v>158</v>
@@ -4487,10 +4487,10 @@
       <c r="C88" t="s">
         <v>23</v>
       </c>
-      <c r="F88" s="49" t="s">
+      <c r="F88" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="G88" s="49"/>
+      <c r="G88" s="48"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
@@ -4503,8 +4503,8 @@
       <c r="D89" t="s">
         <v>117</v>
       </c>
-      <c r="F89" s="49"/>
-      <c r="G89" s="49"/>
+      <c r="F89" s="48"/>
+      <c r="G89" s="48"/>
       <c r="H89" t="s">
         <v>175</v>
       </c>
@@ -4520,8 +4520,8 @@
       <c r="C90" t="s">
         <v>23</v>
       </c>
-      <c r="F90" s="49"/>
-      <c r="G90" s="49"/>
+      <c r="F90" s="48"/>
+      <c r="G90" s="48"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B91" s="23"/>
@@ -4594,10 +4594,10 @@
       <c r="B98" s="22"/>
       <c r="C98" s="20"/>
       <c r="D98" s="27"/>
-      <c r="E98" s="47" t="s">
+      <c r="E98" s="49" t="s">
         <v>168</v>
       </c>
-      <c r="F98" s="47"/>
+      <c r="F98" s="49"/>
       <c r="G98" s="45"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -4748,10 +4748,10 @@
       <c r="C108" t="s">
         <v>42</v>
       </c>
-      <c r="F108" s="49" t="s">
+      <c r="F108" s="48" t="s">
         <v>132</v>
       </c>
-      <c r="G108" s="49"/>
+      <c r="G108" s="48"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
@@ -4770,8 +4770,8 @@
       <c r="E109" t="s">
         <v>124</v>
       </c>
-      <c r="F109" s="49"/>
-      <c r="G109" s="49"/>
+      <c r="F109" s="48"/>
+      <c r="G109" s="48"/>
       <c r="H109" t="s">
         <v>172</v>
       </c>
@@ -4793,8 +4793,8 @@
       <c r="E110" t="s">
         <v>124</v>
       </c>
-      <c r="F110" s="49"/>
-      <c r="G110" s="49"/>
+      <c r="F110" s="48"/>
+      <c r="G110" s="48"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
@@ -4863,10 +4863,10 @@
       <c r="B118" s="22"/>
       <c r="C118" s="20"/>
       <c r="D118" s="27"/>
-      <c r="E118" s="47" t="s">
+      <c r="E118" s="49" t="s">
         <v>168</v>
       </c>
-      <c r="F118" s="47"/>
+      <c r="F118" s="49"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
@@ -5082,10 +5082,10 @@
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F134" s="49" t="s">
+      <c r="F134" s="48" t="s">
         <v>141</v>
       </c>
-      <c r="G134" s="49"/>
+      <c r="G134" s="48"/>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
@@ -5105,8 +5105,8 @@
       <c r="E135" t="s">
         <v>43</v>
       </c>
-      <c r="F135" s="49"/>
-      <c r="G135" s="49"/>
+      <c r="F135" s="48"/>
+      <c r="G135" s="48"/>
       <c r="H135" t="s">
         <v>175</v>
       </c>
@@ -5128,8 +5128,8 @@
       <c r="E136" t="s">
         <v>124</v>
       </c>
-      <c r="F136" s="49"/>
-      <c r="G136" s="49"/>
+      <c r="F136" s="48"/>
+      <c r="G136" s="48"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
@@ -5150,10 +5150,10 @@
       <c r="B140" s="22"/>
       <c r="C140" s="20"/>
       <c r="D140" s="27"/>
-      <c r="E140" s="47" t="s">
+      <c r="E140" s="49" t="s">
         <v>168</v>
       </c>
-      <c r="F140" s="47"/>
+      <c r="F140" s="49"/>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
@@ -5377,6 +5377,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A152:I152"/>
+    <mergeCell ref="A47:I47"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="A29:I29"/>
+    <mergeCell ref="A56:I56"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="E118:F118"/>
+    <mergeCell ref="E140:F140"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="G63:I66"/>
     <mergeCell ref="A130:I130"/>
@@ -5386,14 +5394,6 @@
     <mergeCell ref="F108:G110"/>
     <mergeCell ref="F88:G90"/>
     <mergeCell ref="E98:F98"/>
-    <mergeCell ref="A152:I152"/>
-    <mergeCell ref="A47:I47"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="A29:I29"/>
-    <mergeCell ref="A56:I56"/>
-    <mergeCell ref="E75:F75"/>
-    <mergeCell ref="E118:F118"/>
-    <mergeCell ref="E140:F140"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -7200,11 +7200,11 @@
       </c>
     </row>
     <row r="61" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="G61" s="48" t="s">
+      <c r="G61" s="47" t="s">
         <v>143</v>
       </c>
-      <c r="H61" s="49"/>
-      <c r="I61" s="49"/>
+      <c r="H61" s="48"/>
+      <c r="I61" s="48"/>
     </row>
     <row r="62" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -7216,9 +7216,9 @@
       <c r="C62" t="s">
         <v>79</v>
       </c>
-      <c r="G62" s="49"/>
-      <c r="H62" s="49"/>
-      <c r="I62" s="49"/>
+      <c r="G62" s="48"/>
+      <c r="H62" s="48"/>
+      <c r="I62" s="48"/>
     </row>
     <row r="63" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
@@ -7230,9 +7230,9 @@
       <c r="C63" t="s">
         <v>10</v>
       </c>
-      <c r="G63" s="49"/>
-      <c r="H63" s="49"/>
-      <c r="I63" s="49"/>
+      <c r="G63" s="48"/>
+      <c r="H63" s="48"/>
+      <c r="I63" s="48"/>
     </row>
     <row r="64" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
@@ -7252,9 +7252,9 @@
       <c r="E64" t="s">
         <v>75</v>
       </c>
-      <c r="G64" s="49"/>
-      <c r="H64" s="49"/>
-      <c r="I64" s="49"/>
+      <c r="G64" s="48"/>
+      <c r="H64" s="48"/>
+      <c r="I64" s="48"/>
     </row>
     <row r="65" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
@@ -7524,10 +7524,10 @@
       <c r="C75" t="s">
         <v>23</v>
       </c>
-      <c r="F75" s="49" t="s">
+      <c r="F75" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="G75" s="49"/>
+      <c r="G75" s="48"/>
       <c r="J75" t="s">
         <v>23</v>
       </c>
@@ -7667,8 +7667,8 @@
       <c r="D76" t="s">
         <v>117</v>
       </c>
-      <c r="F76" s="49"/>
-      <c r="G76" s="49"/>
+      <c r="F76" s="48"/>
+      <c r="G76" s="48"/>
     </row>
     <row r="77" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
@@ -7681,8 +7681,8 @@
       <c r="C77" t="s">
         <v>23</v>
       </c>
-      <c r="F77" s="49"/>
-      <c r="G77" s="49"/>
+      <c r="F77" s="48"/>
+      <c r="G77" s="48"/>
     </row>
     <row r="78" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A78" s="46" t="s">
@@ -7731,10 +7731,10 @@
       <c r="C81" t="s">
         <v>42</v>
       </c>
-      <c r="F81" s="49" t="s">
+      <c r="F81" s="48" t="s">
         <v>132</v>
       </c>
-      <c r="G81" s="49"/>
+      <c r="G81" s="48"/>
     </row>
     <row r="82" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
@@ -7753,8 +7753,8 @@
       <c r="E82" t="s">
         <v>124</v>
       </c>
-      <c r="F82" s="49"/>
-      <c r="G82" s="49"/>
+      <c r="F82" s="48"/>
+      <c r="G82" s="48"/>
     </row>
     <row r="83" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
@@ -7773,8 +7773,8 @@
       <c r="E83" t="s">
         <v>124</v>
       </c>
-      <c r="F83" s="49"/>
-      <c r="G83" s="49"/>
+      <c r="F83" s="48"/>
+      <c r="G83" s="48"/>
     </row>
     <row r="85" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
@@ -8515,10 +8515,10 @@
       </c>
     </row>
     <row r="94" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="F94" s="49" t="s">
+      <c r="F94" s="48" t="s">
         <v>141</v>
       </c>
-      <c r="G94" s="49"/>
+      <c r="G94" s="48"/>
     </row>
     <row r="95" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
@@ -8537,8 +8537,8 @@
       <c r="E95" t="s">
         <v>43</v>
       </c>
-      <c r="F95" s="49"/>
-      <c r="G95" s="49"/>
+      <c r="F95" s="48"/>
+      <c r="G95" s="48"/>
     </row>
     <row r="96" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
@@ -8557,8 +8557,8 @@
       <c r="E96" t="s">
         <v>124</v>
       </c>
-      <c r="F96" s="49"/>
-      <c r="G96" s="49"/>
+      <c r="F96" s="48"/>
+      <c r="G96" s="48"/>
     </row>
     <row r="98" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
@@ -8895,12 +8895,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="G61:I64"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A13:I13"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A45:I45"/>
-    <mergeCell ref="A54:I54"/>
     <mergeCell ref="A100:I100"/>
     <mergeCell ref="A74:I74"/>
     <mergeCell ref="F75:G77"/>
@@ -8908,6 +8902,12 @@
     <mergeCell ref="F81:G83"/>
     <mergeCell ref="A90:I90"/>
     <mergeCell ref="F94:G96"/>
+    <mergeCell ref="G61:I64"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A13:I13"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A45:I45"/>
+    <mergeCell ref="A54:I54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>